<commit_message>
Pequeño cambio en el cronograma del proyecto
</commit_message>
<xml_diff>
--- a/Documentación/PLAN_DEL_PROYECTO.xlsx
+++ b/Documentación/PLAN_DEL_PROYECTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LILY\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A5B880E-AC8C-4078-86E9-AF561EA46EAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA2FE78-51E2-4911-9C6D-8CB88E3112F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="109">
   <si>
     <t>Actividades del proyecto</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Andrea Ospina</t>
-  </si>
-  <si>
-    <t>Project manager</t>
   </si>
   <si>
     <t>Actividad</t>
@@ -505,7 +502,7 @@
     <numFmt numFmtId="164" formatCode="d"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -597,6 +594,20 @@
       <sz val="16"/>
       <color rgb="FF777777"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF777777"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -845,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -942,13 +953,17 @@
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1404,7 +1419,7 @@
     <row r="2" spans="1:39" ht="63.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:39" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B3" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="23.25" x14ac:dyDescent="0.25">
@@ -1413,8 +1428,8 @@
       </c>
     </row>
     <row r="5" spans="1:39" ht="21" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
-        <v>109</v>
+      <c r="B5" s="40" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1690,10 +1705,10 @@
       <c r="D9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="43"/>
       <c r="I9" s="16"/>
       <c r="K9" s="16"/>
       <c r="P9" s="16"/>
@@ -1765,22 +1780,22 @@
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="41"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="44"/>
       <c r="W11" s="16"/>
       <c r="Y11" s="16"/>
       <c r="AD11" s="16"/>
@@ -1800,22 +1815,22 @@
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="40"/>
-      <c r="T12" s="40"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
       <c r="W12" s="17"/>
@@ -1875,21 +1890,21 @@
       <c r="E14" s="15"/>
       <c r="F14" s="14"/>
       <c r="G14" s="25"/>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
       <c r="W14" s="17"/>
@@ -1926,11 +1941,11 @@
       <c r="K15" s="16"/>
       <c r="P15" s="16"/>
       <c r="R15" s="16"/>
-      <c r="T15" s="42" t="s">
+      <c r="T15" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="U15" s="42"/>
-      <c r="V15" s="42"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
       <c r="W15" s="16"/>
       <c r="Y15" s="16"/>
       <c r="AD15" s="16"/>
@@ -1964,10 +1979,10 @@
       <c r="R16" s="17"/>
       <c r="S16" s="13"/>
       <c r="T16" s="26"/>
-      <c r="U16" s="43" t="s">
+      <c r="U16" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="V16" s="43"/>
+      <c r="V16" s="41"/>
       <c r="W16" s="17"/>
       <c r="X16" s="13"/>
       <c r="Y16" s="17"/>
@@ -2002,10 +2017,10 @@
       <c r="K17" s="16"/>
       <c r="P17" s="16"/>
       <c r="R17" s="16"/>
-      <c r="W17" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="X17" s="44"/>
+      <c r="W17" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="X17" s="42"/>
       <c r="Y17" s="16"/>
       <c r="AD17" s="16"/>
       <c r="AF17" s="16"/>
@@ -2043,7 +2058,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="28"/>
       <c r="Y18" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Z18" s="13"/>
       <c r="AA18" s="13"/>
@@ -2084,8 +2099,8 @@
   </sheetPr>
   <dimension ref="A2:L84"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J79" sqref="J79"/>
+    <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,7 +2118,7 @@
     <row r="2" spans="1:12" ht="63.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B3" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
@@ -2112,9 +2127,12 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B5" s="39">
-        <v>44019.800869375002</v>
-      </c>
+      <c r="B5" s="39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="46"/>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
@@ -2146,42 +2164,42 @@
       <c r="B11" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>28</v>
+      <c r="C11" s="47" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
       <c r="B16" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>30</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
       <c r="F16" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
       <c r="I16" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="K16" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="L16" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="L16" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
       <c r="B18" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -2196,22 +2214,22 @@
     </row>
     <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="G19" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="I19" s="33" t="s">
         <v>40</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>41</v>
       </c>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
@@ -2222,10 +2240,10 @@
         <v>27</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I20" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J20" s="33"/>
       <c r="K20" s="33"/>
@@ -2234,7 +2252,7 @@
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -2249,22 +2267,22 @@
     </row>
     <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="33" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>45</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>46</v>
       </c>
       <c r="J24" s="33"/>
       <c r="K24" s="33"/>
@@ -2275,10 +2293,10 @@
         <v>27</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J25" s="33"/>
       <c r="K25" s="33"/>
@@ -2287,7 +2305,7 @@
     <row r="28" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="30"/>
       <c r="B28" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
@@ -2302,25 +2320,25 @@
     </row>
     <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F29" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="33" t="s">
         <v>50</v>
-      </c>
-      <c r="G29" t="s">
-        <v>38</v>
-      </c>
-      <c r="I29" s="33" t="s">
-        <v>51</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K29" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L29" s="33"/>
     </row>
@@ -2329,128 +2347,128 @@
         <v>27</v>
       </c>
       <c r="G30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I30" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J30" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L30" s="33"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I31" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J31" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K31" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L31" s="33"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I32" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L32" s="33"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I33" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J33" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K33" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L33" s="33"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I34" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K34" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L34" s="33"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I35" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J35" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K35" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L35" s="33"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K36" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L36" s="33"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I37" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J37" s="33" t="s">
         <v>27</v>
       </c>
       <c r="K37" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L37" s="33"/>
     </row>
     <row r="40" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="30"/>
       <c r="B40" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="30"/>
@@ -2465,19 +2483,19 @@
     </row>
     <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I41" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J41" s="33"/>
       <c r="K41" s="33"/>
@@ -2488,10 +2506,10 @@
         <v>27</v>
       </c>
       <c r="G42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I42" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J42" s="33"/>
       <c r="K42" s="33"/>
@@ -2499,10 +2517,10 @@
     </row>
     <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I43" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J43" s="33"/>
       <c r="K43" s="33"/>
@@ -2511,7 +2529,7 @@
     <row r="46" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="30"/>
       <c r="B46" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" s="30"/>
       <c r="D46" s="30"/>
@@ -2526,22 +2544,22 @@
     </row>
     <row r="47" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B47" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="33" t="s">
         <v>25</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F47" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" t="s">
+        <v>37</v>
+      </c>
+      <c r="I47" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="G47" t="s">
-        <v>38</v>
-      </c>
-      <c r="I47" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="J47" s="33"/>
       <c r="K47" s="33"/>
@@ -2552,10 +2570,10 @@
         <v>27</v>
       </c>
       <c r="G48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I48" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J48" s="33"/>
       <c r="K48" s="33"/>
@@ -2564,7 +2582,7 @@
     <row r="51" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="30"/>
       <c r="B51" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
@@ -2579,25 +2597,25 @@
     </row>
     <row r="52" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B52" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C52" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F52" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I52" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J52" s="33" t="s">
         <v>25</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L52" s="33"/>
     </row>
@@ -2606,40 +2624,40 @@
         <v>27</v>
       </c>
       <c r="G53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I53" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J53" s="33" t="s">
         <v>25</v>
       </c>
       <c r="K53" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L53" s="33"/>
     </row>
     <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I54" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J54" s="33" t="s">
         <v>25</v>
       </c>
       <c r="K54" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L54" s="33"/>
     </row>
     <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I55" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J55" s="33" t="s">
         <v>25</v>
@@ -2649,10 +2667,10 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I56" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J56" s="33" t="s">
         <v>25</v>
@@ -2662,70 +2680,70 @@
     </row>
     <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I57" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J57" s="33" t="s">
         <v>25</v>
       </c>
       <c r="K57" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L57" s="33"/>
     </row>
     <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I58" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J58" s="33" t="s">
         <v>25</v>
       </c>
       <c r="K58" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L58" s="33"/>
     </row>
     <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I59" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J59" s="33" t="s">
         <v>25</v>
       </c>
       <c r="K59" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L59" s="33"/>
     </row>
     <row r="60" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I60" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J60" s="33" t="s">
         <v>25</v>
       </c>
       <c r="K60" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L60" s="33"/>
     </row>
     <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I61" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J61" s="33" t="s">
         <v>25</v>
@@ -2736,7 +2754,7 @@
     <row r="64" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A64" s="30"/>
       <c r="B64" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C64" s="30"/>
       <c r="D64" s="30"/>
@@ -2751,19 +2769,19 @@
     </row>
     <row r="65" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F65" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I65" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J65" s="33"/>
       <c r="K65" s="33"/>
@@ -2774,10 +2792,10 @@
         <v>27</v>
       </c>
       <c r="G66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I66" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J66" s="33"/>
       <c r="K66" s="33"/>
@@ -2785,10 +2803,10 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I67" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J67" s="33"/>
       <c r="K67" s="33"/>
@@ -2797,7 +2815,7 @@
     <row r="70" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="30"/>
       <c r="B70" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C70" s="30"/>
       <c r="D70" s="30"/>
@@ -2812,19 +2830,19 @@
     </row>
     <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C71" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F71" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I71" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J71" s="33"/>
       <c r="K71" s="33"/>
@@ -2838,7 +2856,7 @@
     <row r="75" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A75" s="30"/>
       <c r="B75" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C75" s="30"/>
       <c r="D75" s="30"/>
@@ -2853,19 +2871,19 @@
     </row>
     <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B76" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C76" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F76" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G76" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I76" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J76" s="33"/>
       <c r="K76" s="33"/>
@@ -2876,10 +2894,10 @@
         <v>27</v>
       </c>
       <c r="G77" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I77" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J77" s="33"/>
       <c r="K77" s="33"/>
@@ -2887,10 +2905,10 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I78" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J78" s="33"/>
       <c r="K78" s="33"/>
@@ -2898,10 +2916,10 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I79" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J79" s="33"/>
       <c r="K79" s="33"/>
@@ -2925,16 +2943,16 @@
     </row>
     <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C83" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F83" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I83" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -2945,7 +2963,7 @@
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>